<commit_message>
Updated the template and adjusted the latest result files accordingly
</commit_message>
<xml_diff>
--- a/17.xlsx
+++ b/17.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bfarleigh1\Desktop\FPix\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15160" windowHeight="20560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$N$80</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="99">
   <si>
     <t>Test all connections listed in the table below and record the values observed. Use the test points on the adapter board.</t>
   </si>
@@ -230,9 +225,6 @@
     <t>Final decision:</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>1) Do not connect the adapter. Turn HV on, read after 60 sec</t>
   </si>
   <si>
@@ -323,10 +315,10 @@
     <t>PSI</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>Corrected</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -436,8 +428,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="181">
+  <cellStyleXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -712,7 +722,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="181">
+  <cellStyles count="199">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -803,6 +813,15 @@
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -893,6 +912,15 @@
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1241,71 +1269,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="8.375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.875" style="9"/>
-    <col min="6" max="6" width="10.875" style="5"/>
-    <col min="9" max="9" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="9"/>
+    <col min="6" max="6" width="11" style="5"/>
+    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.875" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="26.25">
       <c r="A1" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="32"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="B4" s="28"/>
       <c r="C4" s="5">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="28"/>
       <c r="C5" s="29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="28"/>
       <c r="C6" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="31">
         <v>79980109</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H6" s="27">
         <v>0.1</v>
@@ -1314,40 +1342,40 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" s="31">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="28"/>
       <c r="C8" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="31">
         <v>1268080</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15">
       <c r="B9" s="28"/>
       <c r="C9" s="21"/>
     </row>
-    <row r="11" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1355,7 +1383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1363,17 +1391,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="B15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="O16" s="18" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
@@ -1411,7 +1439,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1440,20 +1468,21 @@
       <c r="J18" t="s">
         <v>13</v>
       </c>
+      <c r="K18" s="12"/>
       <c r="L18" s="9" t="str">
-        <f t="shared" ref="L18:L33" si="0">IF(K18&lt;K$34,"ok","NOK")</f>
-        <v>ok</v>
+        <f>IF(AND(K18&lt;K$34,ISNUMBER(K18)),"ok","NOK")</f>
+        <v>NOK</v>
       </c>
       <c r="O18">
-        <f t="shared" ref="O18:O51" si="1">IF(G18="NOK",1,0)</f>
+        <f t="shared" ref="O18:O51" si="0">IF(G18="NOK",1,0)</f>
         <v>0</v>
       </c>
       <c r="P18">
         <f>IF(L18="NOK",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1482,20 +1511,21 @@
       <c r="J19" t="s">
         <v>14</v>
       </c>
+      <c r="K19" s="12"/>
       <c r="L19" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" ref="L19:L33" si="1">IF(AND(K19&lt;K$34,ISNUMBER(K19)),"ok","NOK")</f>
+        <v>NOK</v>
       </c>
       <c r="O19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P19">
         <f t="shared" ref="P19:P33" si="2">IF(L19="NOK",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1525,20 +1555,21 @@
       <c r="J20" t="s">
         <v>9</v>
       </c>
+      <c r="K20" s="12"/>
       <c r="L20" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
       <c r="O20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P20">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1568,20 +1599,21 @@
       <c r="J21" t="s">
         <v>9</v>
       </c>
+      <c r="K21" s="12"/>
       <c r="L21" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
       <c r="O21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P21">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1610,20 +1642,21 @@
       <c r="J22" t="s">
         <v>15</v>
       </c>
+      <c r="K22" s="12"/>
       <c r="L22" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
       <c r="O22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P22">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1652,20 +1685,21 @@
       <c r="J23" t="s">
         <v>16</v>
       </c>
+      <c r="K23" s="12"/>
       <c r="L23" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
       <c r="O23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P23">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1694,20 +1728,21 @@
       <c r="J24" t="s">
         <v>17</v>
       </c>
+      <c r="K24" s="12"/>
       <c r="L24" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
       <c r="O24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P24">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1736,20 +1771,21 @@
       <c r="J25" t="s">
         <v>18</v>
       </c>
+      <c r="K25" s="12"/>
       <c r="L25" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
       <c r="O25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P25">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1778,20 +1814,21 @@
       <c r="J26" t="s">
         <v>19</v>
       </c>
+      <c r="K26" s="12"/>
       <c r="L26" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
       <c r="O26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P26">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1820,20 +1857,21 @@
       <c r="J27" t="s">
         <v>20</v>
       </c>
+      <c r="K27" s="12"/>
       <c r="L27" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
       <c r="O27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P27">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1862,20 +1900,21 @@
       <c r="J28" t="s">
         <v>21</v>
       </c>
+      <c r="K28" s="12"/>
       <c r="L28" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
       <c r="O28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P28">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1904,20 +1943,21 @@
       <c r="J29" t="s">
         <v>22</v>
       </c>
+      <c r="K29" s="12"/>
       <c r="L29" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
       <c r="O29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P29">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1946,20 +1986,21 @@
       <c r="J30" t="s">
         <v>10</v>
       </c>
+      <c r="K30" s="12"/>
       <c r="L30" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
       <c r="O30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P30">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1988,20 +2029,21 @@
       <c r="J31" t="s">
         <v>10</v>
       </c>
+      <c r="K31" s="12"/>
       <c r="L31" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
       <c r="O31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P31">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -2031,20 +2073,21 @@
       <c r="J32" t="s">
         <v>11</v>
       </c>
+      <c r="K32" s="12"/>
       <c r="L32" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
       <c r="O32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P32">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -2073,20 +2116,21 @@
       <c r="J33" t="s">
         <v>12</v>
       </c>
+      <c r="K33" s="12"/>
       <c r="L33" s="9" t="str">
-        <f t="shared" si="0"/>
-        <v>ok</v>
+        <f t="shared" si="1"/>
+        <v>NOK</v>
       </c>
       <c r="O33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P33">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -2117,11 +2161,11 @@
         <v>1</v>
       </c>
       <c r="O34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -2147,11 +2191,11 @@
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -2184,11 +2228,11 @@
       <c r="M36" s="18"/>
       <c r="N36" s="18"/>
       <c r="O36">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -2217,11 +2261,11 @@
       <c r="J37" s="18"/>
       <c r="K37" s="18"/>
       <c r="O37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>19</v>
       </c>
@@ -2246,11 +2290,11 @@
         <v>ok</v>
       </c>
       <c r="O38">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -2286,11 +2330,11 @@
         <v>7</v>
       </c>
       <c r="O39">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -2320,20 +2364,21 @@
       <c r="J40" t="s">
         <v>8</v>
       </c>
+      <c r="K40" s="12"/>
       <c r="L40" s="9" t="str">
-        <f>IF(K40&lt;K$48,"ok","NOK")</f>
-        <v>ok</v>
+        <f>IF(AND(K40&lt;K$48,ISNUMBER(K40)),"ok","NOK")</f>
+        <v>NOK</v>
       </c>
       <c r="O40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P40">
         <f t="shared" ref="P40:P47" si="5">IF(L40="NOK",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -2363,20 +2408,21 @@
       <c r="J41" t="s">
         <v>8</v>
       </c>
+      <c r="K41" s="12"/>
       <c r="L41" s="9" t="str">
-        <f t="shared" ref="L41:L47" si="6">IF(K41&lt;K$48,"ok","NOK")</f>
-        <v>ok</v>
+        <f t="shared" ref="L41:L47" si="6">IF(AND(K41&lt;K$48,ISNUMBER(K41)),"ok","NOK")</f>
+        <v>NOK</v>
       </c>
       <c r="O41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P41">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>28</v>
       </c>
@@ -2406,20 +2452,21 @@
       <c r="J42" t="s">
         <v>9</v>
       </c>
+      <c r="K42" s="12"/>
       <c r="L42" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>ok</v>
+        <v>NOK</v>
       </c>
       <c r="O42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P42">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -2450,20 +2497,21 @@
       <c r="J43" t="s">
         <v>8</v>
       </c>
+      <c r="K43" s="12"/>
       <c r="L43" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>ok</v>
+        <v>NOK</v>
       </c>
       <c r="O43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P43">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44" t="s">
         <v>32</v>
       </c>
@@ -2494,20 +2542,21 @@
       <c r="J44" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="K44" s="12"/>
       <c r="L44" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>ok</v>
+        <v>NOK</v>
       </c>
       <c r="O44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P44">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -2538,20 +2587,21 @@
       <c r="J45" t="s">
         <v>10</v>
       </c>
+      <c r="K45" s="12"/>
       <c r="L45" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>ok</v>
+        <v>NOK</v>
       </c>
       <c r="O45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P45">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -2581,20 +2631,21 @@
       <c r="J46" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="K46" s="12"/>
       <c r="L46" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>ok</v>
+        <v>NOK</v>
       </c>
       <c r="O46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P46">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -2623,20 +2674,21 @@
       <c r="J47" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="K47" s="12"/>
       <c r="L47" s="9" t="str">
         <f t="shared" si="6"/>
-        <v>ok</v>
+        <v>NOK</v>
       </c>
       <c r="O47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P47">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -2666,11 +2718,11 @@
         <v>0.5</v>
       </c>
       <c r="O48">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -2694,11 +2746,11 @@
         <v>ok</v>
       </c>
       <c r="O49">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -2728,11 +2780,11 @@
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
       <c r="O50">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -2762,34 +2814,34 @@
       <c r="K51" s="21"/>
       <c r="L51" s="21"/>
       <c r="O51">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53" t="s">
         <v>40</v>
       </c>
       <c r="B53" s="14" t="str">
         <f>IF(SUM(O18:O51,P18:P33,P40:P47)&gt;0,"FAIL","PASS")</f>
-        <v>PASS</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="18.75">
       <c r="A55" s="1" t="s">
         <v>37</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15">
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -2797,15 +2849,15 @@
         <v>38</v>
       </c>
       <c r="I57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J57" s="14"/>
       <c r="K57" s="5"/>
       <c r="M57" s="31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
         <v>3</v>
       </c>
@@ -2813,38 +2865,36 @@
         <v>43</v>
       </c>
       <c r="I58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J58" s="14"/>
       <c r="K58" s="5"/>
       <c r="M58" s="31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="I59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J59" s="14"/>
       <c r="K59" s="5"/>
       <c r="M59" s="31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
         <v>39</v>
       </c>
-      <c r="B60" s="24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B60" s="24"/>
+    </row>
+    <row r="62" spans="1:15" ht="18.75">
       <c r="A62" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15">
       <c r="A64" t="s">
         <v>1</v>
       </c>
@@ -2852,10 +2902,10 @@
         <v>42</v>
       </c>
       <c r="I64" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
       <c r="A65" t="s">
         <v>3</v>
       </c>
@@ -2863,86 +2913,94 @@
         <v>44</v>
       </c>
       <c r="I65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J65" s="25"/>
       <c r="K65" s="17"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13">
       <c r="B66" t="s">
+        <v>67</v>
+      </c>
+      <c r="I66" t="s">
+        <v>85</v>
+      </c>
+      <c r="K66" s="33">
+        <v>98.8</v>
+      </c>
+      <c r="L66" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M66" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="B67" t="s">
         <v>68</v>
       </c>
-      <c r="I66" t="s">
-        <v>86</v>
-      </c>
-      <c r="K66" s="33"/>
-      <c r="L66" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="M66" s="18" t="s">
+      <c r="I67" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>69</v>
-      </c>
-      <c r="I67" t="s">
-        <v>89</v>
-      </c>
-      <c r="K67" s="33"/>
+      <c r="K67" s="33">
+        <v>9.92</v>
+      </c>
       <c r="L67" s="5" t="s">
         <v>45</v>
       </c>
       <c r="M67" s="18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
       <c r="B68" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
       <c r="I69" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K69" s="34">
         <f>102000*K67*0.000001</f>
-        <v>0</v>
+        <v>1.0118399999999999</v>
       </c>
       <c r="L69" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
       <c r="B70" t="s">
-        <v>71</v>
-      </c>
-      <c r="C70" s="25"/>
+        <v>70</v>
+      </c>
+      <c r="C70" s="25">
+        <v>1.7000000000000001E-2</v>
+      </c>
       <c r="D70" s="4" t="s">
         <v>45</v>
       </c>
       <c r="I70" s="26" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
       <c r="B71" t="s">
-        <v>72</v>
-      </c>
-      <c r="C71" s="25"/>
+        <v>71</v>
+      </c>
+      <c r="C71" s="25">
+        <v>2.5999999999999999E-2</v>
+      </c>
       <c r="D71" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13">
       <c r="B72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C72" s="25">
         <f>C71-C70</f>
-        <v>0</v>
+        <v>8.9999999999999976E-3</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>45</v>
@@ -2957,39 +3015,39 @@
         <v>45</v>
       </c>
       <c r="I72" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K72" s="19">
         <f>K66+K69</f>
-        <v>0</v>
+        <v>99.811840000000004</v>
       </c>
       <c r="L72" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
       <c r="C73" s="25"/>
       <c r="D73" s="17"/>
       <c r="G73" s="26"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13">
       <c r="C74" s="25"/>
       <c r="D74" s="4"/>
       <c r="G74" s="26"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13">
       <c r="A75" t="s">
         <v>39</v>
       </c>
       <c r="B75" s="14" t="str">
         <f>IF(AND(C72&lt;=F72,ABS(K72-100)&lt;0.5),"PASS","FAIL")</f>
-        <v>FAIL</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+        <v>PASS</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
       <c r="B77" s="14"/>
     </row>
-    <row r="78" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" ht="18.75">
       <c r="A78" s="1" t="s">
         <v>66</v>
       </c>
@@ -2999,7 +3057,7 @@
         <v>REJECTED</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -3020,7 +3078,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.43000000000000005" right="0.43000000000000005" top="0.51181102362204722" bottom="0.43000000000000005" header="0.43000000000000005" footer="0.43000000000000005"/>
-  <pageSetup paperSize="9" scale="60" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="60" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>